<commit_message>
new key-value pairs added
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\divek\Documents\GitHub\Inclusive-Language-using-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925F6DFB-BD03-43A6-8358-282C55C2F0E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DA4E3B-5409-40E5-82D9-A9EC00D19FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="18" xr2:uid="{20A34141-9B13-4300-9F48-2DF660D6B3BA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{20A34141-9B13-4300-9F48-2DF660D6B3BA}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <sheet name="Y" sheetId="25" r:id="rId25"/>
     <sheet name="Z" sheetId="26" r:id="rId26"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,6 +50,7 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="476">
   <si>
     <t>KEY</t>
   </si>
@@ -428,9 +429,6 @@
     <t>Mentally ill</t>
   </si>
   <si>
-    <t>has a mental illness</t>
-  </si>
-  <si>
     <t>Substance abuse disorder</t>
   </si>
   <si>
@@ -980,9 +978,6 @@
     <t>Oriental</t>
   </si>
   <si>
-    <t>Asain</t>
-  </si>
-  <si>
     <t>Third-world country</t>
   </si>
   <si>
@@ -1022,9 +1017,6 @@
     <t>Salesman</t>
   </si>
   <si>
-    <t xml:space="preserve">sales representative </t>
-  </si>
-  <si>
     <t>Manmade</t>
   </si>
   <si>
@@ -1050,6 +1042,450 @@
   </si>
   <si>
     <t>Sibling</t>
+  </si>
+  <si>
+    <t>Female Engineer</t>
+  </si>
+  <si>
+    <t>a woman on the engineering team</t>
+  </si>
+  <si>
+    <t>Abusive Relationship</t>
+  </si>
+  <si>
+    <t>relationship with a person who is abusive</t>
+  </si>
+  <si>
+    <t>Prostitute</t>
+  </si>
+  <si>
+    <t>person who engages in sex work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prisoner </t>
+  </si>
+  <si>
+    <t xml:space="preserve">person who is incarcerated </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convict </t>
+  </si>
+  <si>
+    <t>person who has been incarcerated</t>
+  </si>
+  <si>
+    <t>Special needs</t>
+  </si>
+  <si>
+    <t>person with a disability</t>
+  </si>
+  <si>
+    <t>Physically challenged</t>
+  </si>
+  <si>
+    <t>person who has a disability</t>
+  </si>
+  <si>
+    <t>Mentally challenged</t>
+  </si>
+  <si>
+    <t>person with intellectual disability</t>
+  </si>
+  <si>
+    <t>Mentally retarted</t>
+  </si>
+  <si>
+    <t>person with a mental illness</t>
+  </si>
+  <si>
+    <t>Visually-challenged person</t>
+  </si>
+  <si>
+    <t>person who is blind/visually impaired person</t>
+  </si>
+  <si>
+    <t>Sight-challenged person</t>
+  </si>
+  <si>
+    <t>AIDS Victim</t>
+  </si>
+  <si>
+    <t>person with AIDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brain damaged </t>
+  </si>
+  <si>
+    <t>person with a traumatic brain injury</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meth addict </t>
+  </si>
+  <si>
+    <t>person with substance use disorder</t>
+  </si>
+  <si>
+    <t>Birth Sex</t>
+  </si>
+  <si>
+    <t>assigned sex</t>
+  </si>
+  <si>
+    <t>Natal sex</t>
+  </si>
+  <si>
+    <t>sex assigned at birth</t>
+  </si>
+  <si>
+    <t>Low-class people</t>
+  </si>
+  <si>
+    <t>people whose income are below the federal poverty threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Killing it </t>
+  </si>
+  <si>
+    <t>great job!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take a shot at </t>
+  </si>
+  <si>
+    <t>give it  a go</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pull the trigger </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go off the reservation </t>
+  </si>
+  <si>
+    <t>disagree with the group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commited suicide </t>
+  </si>
+  <si>
+    <t xml:space="preserve">died by suicide </t>
+  </si>
+  <si>
+    <t>Completed suicide</t>
+  </si>
+  <si>
+    <t>suicided</t>
+  </si>
+  <si>
+    <t>Child prostitute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">child who has been trafficked </t>
+  </si>
+  <si>
+    <t>Nonconsensual sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rape </t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>Caucasian</t>
+  </si>
+  <si>
+    <t>European american</t>
+  </si>
+  <si>
+    <t>Indigenous people/Native American</t>
+  </si>
+  <si>
+    <t>Eskimos</t>
+  </si>
+  <si>
+    <t>Inuit</t>
+  </si>
+  <si>
+    <t>Tradesman</t>
+  </si>
+  <si>
+    <t>Tradesperson</t>
+  </si>
+  <si>
+    <t>Manned</t>
+  </si>
+  <si>
+    <t>Staffed</t>
+  </si>
+  <si>
+    <t>Businessman</t>
+  </si>
+  <si>
+    <t>Businesswoman</t>
+  </si>
+  <si>
+    <t>Business executive</t>
+  </si>
+  <si>
+    <t>Birth defect</t>
+  </si>
+  <si>
+    <t>person born with a disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Congenital defect </t>
+  </si>
+  <si>
+    <t>person who has a congenital disability</t>
+  </si>
+  <si>
+    <t>Birth deformity</t>
+  </si>
+  <si>
+    <t>Confined to a wheelchair</t>
+  </si>
+  <si>
+    <t>person who uses a wheelchair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hard of hearing </t>
+  </si>
+  <si>
+    <t>person who is hard of hearing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hearing impaired </t>
+  </si>
+  <si>
+    <t>Deaf-mute</t>
+  </si>
+  <si>
+    <t>Epileptic</t>
+  </si>
+  <si>
+    <t>person who has epilepsy</t>
+  </si>
+  <si>
+    <t>Handicapped parking</t>
+  </si>
+  <si>
+    <t>accessible parking</t>
+  </si>
+  <si>
+    <t>Handicapped bathrooms</t>
+  </si>
+  <si>
+    <t>accessible bathrooms</t>
+  </si>
+  <si>
+    <t>Fit,attack,spell</t>
+  </si>
+  <si>
+    <t>Seizure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inarticulate </t>
+  </si>
+  <si>
+    <t>Incoherent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">person who has a speech disorder </t>
+  </si>
+  <si>
+    <t>person who has a speech disability</t>
+  </si>
+  <si>
+    <t>Neurotic</t>
+  </si>
+  <si>
+    <t>person with a mental-health disability</t>
+  </si>
+  <si>
+    <t>Dyslexic</t>
+  </si>
+  <si>
+    <t>person with a learning disability</t>
+  </si>
+  <si>
+    <t>Learning disabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learning disordered </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spastic </t>
+  </si>
+  <si>
+    <t>person who has spasms</t>
+  </si>
+  <si>
+    <t>Suffers from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stricken with </t>
+  </si>
+  <si>
+    <t>afflicted by</t>
+  </si>
+  <si>
+    <t>Victim of cerebral palsy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">person who has cerebral palsy/person with a mobility impairment </t>
+  </si>
+  <si>
+    <t>Manning the office</t>
+  </si>
+  <si>
+    <t>staffing the office</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forefathers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ancestors </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working hours </t>
+  </si>
+  <si>
+    <t xml:space="preserve">man hours </t>
+  </si>
+  <si>
+    <t>Policeman</t>
+  </si>
+  <si>
+    <t>Policewoman</t>
+  </si>
+  <si>
+    <t>Police officer</t>
+  </si>
+  <si>
+    <t>Spokesman</t>
+  </si>
+  <si>
+    <t>Spokesperson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maternity leave </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parental leave </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paternal leave </t>
+  </si>
+  <si>
+    <t>Parental leave/Parental time off</t>
+  </si>
+  <si>
+    <t>Landlord</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>Boyfriend</t>
+  </si>
+  <si>
+    <t>partner</t>
+  </si>
+  <si>
+    <t>Girlfriend</t>
+  </si>
+  <si>
+    <t>sales representative /salesperson</t>
+  </si>
+  <si>
+    <t>Maiden name</t>
+  </si>
+  <si>
+    <t>family name</t>
+  </si>
+  <si>
+    <t>Fireman</t>
+  </si>
+  <si>
+    <t>firefighter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Husband </t>
+  </si>
+  <si>
+    <t xml:space="preserve">spouse </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wife </t>
+  </si>
+  <si>
+    <t>Bad Guy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suspect </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleaning lady </t>
+  </si>
+  <si>
+    <t>Housekeeper</t>
+  </si>
+  <si>
+    <t>Garbage Man</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sanitation engineer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male nurse </t>
+  </si>
+  <si>
+    <t>Nurse</t>
+  </si>
+  <si>
+    <t>Mansplaining</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patronizing </t>
+  </si>
+  <si>
+    <t>Average man</t>
+  </si>
+  <si>
+    <t>average person/ordinary person</t>
+  </si>
+  <si>
+    <t>Layman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layperson </t>
+  </si>
+  <si>
+    <t>To man</t>
+  </si>
+  <si>
+    <t>to operate/to staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Workmanlike </t>
+  </si>
+  <si>
+    <t>skillfull</t>
+  </si>
+  <si>
+    <t>Grooming</t>
+  </si>
+  <si>
+    <t>Refining</t>
+  </si>
+  <si>
+    <t>Straight</t>
+  </si>
+  <si>
+    <t>non-LGBTQ</t>
   </si>
 </sst>
 </file>
@@ -1423,15 +1859,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6858CDCC-8F19-4C26-BB84-3C886140036A}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" customWidth="1"/>
+    <col min="1" max="1" width="19.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1452,66 +1888,98 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" t="s">
         <v>154</v>
-      </c>
-      <c r="B4" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" t="s">
         <v>177</v>
-      </c>
-      <c r="B5" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" t="s">
         <v>192</v>
-      </c>
-      <c r="B6" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B7" t="s">
         <v>222</v>
-      </c>
-      <c r="B7" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8" t="s">
         <v>224</v>
-      </c>
-      <c r="B8" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>233</v>
+      </c>
+      <c r="B9" t="s">
         <v>234</v>
-      </c>
-      <c r="B9" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B10" t="s">
         <v>244</v>
       </c>
-      <c r="B10" t="s">
-        <v>245</v>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>330</v>
+      </c>
+      <c r="B11" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>349</v>
+      </c>
+      <c r="B12" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>423</v>
+      </c>
+      <c r="B13" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>464</v>
+      </c>
+      <c r="B14" t="s">
+        <v>465</v>
       </c>
     </row>
   </sheetData>
@@ -1544,10 +2012,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8141D833-7611-4242-9B00-E47F9E6D638A}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1565,18 +2033,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B2" t="s">
         <v>261</v>
-      </c>
-      <c r="B2" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B3" t="s">
         <v>263</v>
       </c>
-      <c r="B3" t="s">
-        <v>264</v>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>361</v>
+      </c>
+      <c r="B4" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -1586,10 +2062,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C043F532-906E-4302-9FB6-256AACBA4087}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1623,18 +2099,58 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" t="s">
         <v>265</v>
-      </c>
-      <c r="B4" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B5" t="s">
         <v>298</v>
       </c>
-      <c r="B5" t="s">
-        <v>299</v>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>359</v>
+      </c>
+      <c r="B6" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>417</v>
+      </c>
+      <c r="B7" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>418</v>
+      </c>
+      <c r="B8" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>441</v>
+      </c>
+      <c r="B9" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>466</v>
+      </c>
+      <c r="B10" t="s">
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -1644,10 +2160,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09836E84-368E-489C-9D89-DF2EE8B16D2B}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1741,95 +2257,167 @@
         <v>122</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>345</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>149</v>
+      </c>
+      <c r="B13" t="s">
         <v>150</v>
-      </c>
-      <c r="B13" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14" t="s">
         <v>173</v>
-      </c>
-      <c r="B14" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>183</v>
+      </c>
+      <c r="B15" t="s">
         <v>184</v>
-      </c>
-      <c r="B15" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>207</v>
+      </c>
+      <c r="B16" t="s">
         <v>208</v>
-      </c>
-      <c r="B16" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>229</v>
+      </c>
+      <c r="B17" t="s">
         <v>230</v>
-      </c>
-      <c r="B17" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>237</v>
+      </c>
+      <c r="B18" t="s">
         <v>238</v>
-      </c>
-      <c r="B18" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>239</v>
+      </c>
+      <c r="B19" t="s">
         <v>240</v>
-      </c>
-      <c r="B19" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>286</v>
+      </c>
+      <c r="B20" t="s">
         <v>287</v>
-      </c>
-      <c r="B20" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>303</v>
+      </c>
+      <c r="B21" t="s">
         <v>304</v>
-      </c>
-      <c r="B21" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B22" t="s">
-        <v>323</v>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>342</v>
+      </c>
+      <c r="B23" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>344</v>
+      </c>
+      <c r="B24" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>353</v>
+      </c>
+      <c r="B25" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>385</v>
+      </c>
+      <c r="B26" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>426</v>
+      </c>
+      <c r="B27" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>437</v>
+      </c>
+      <c r="B28" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>447</v>
+      </c>
+      <c r="B29" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>460</v>
+      </c>
+      <c r="B30" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>462</v>
+      </c>
+      <c r="B31" t="s">
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -1839,15 +2427,15 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F643455A-BF54-40F7-A3F8-8EAD8E02FB93}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1876,62 +2464,87 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" t="s">
         <v>210</v>
-      </c>
-      <c r="B5" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" t="s">
         <v>267</v>
-      </c>
-      <c r="B6" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>268</v>
+      </c>
+      <c r="B7" t="s">
         <v>269</v>
-      </c>
-      <c r="B7" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>301</v>
+      </c>
+      <c r="B8" t="s">
         <v>302</v>
-      </c>
-      <c r="B8" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B9" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B10" t="s">
-        <v>326</v>
+        <v>323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>357</v>
+      </c>
+      <c r="B11" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>375</v>
+      </c>
+      <c r="B12" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>413</v>
+      </c>
+      <c r="B13" t="s">
+        <v>414</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1940,7 +2553,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1958,26 +2571,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2" t="s">
         <v>271</v>
-      </c>
-      <c r="B2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B3" t="s">
         <v>273</v>
-      </c>
-      <c r="B3" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B4" t="s">
-        <v>307</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -1987,15 +2600,15 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20CA873D-6197-48F6-A494-2FF335502137}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -2024,34 +2637,90 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" t="s">
         <v>126</v>
-      </c>
-      <c r="B4" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>274</v>
+      </c>
+      <c r="B6" t="s">
         <v>275</v>
-      </c>
-      <c r="B6" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B7" t="s">
-        <v>318</v>
+        <v>316</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>332</v>
+      </c>
+      <c r="B8" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>334</v>
+      </c>
+      <c r="B9" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>340</v>
+      </c>
+      <c r="B10" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>365</v>
+      </c>
+      <c r="B11" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>432</v>
+      </c>
+      <c r="B12" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>433</v>
+      </c>
+      <c r="B13" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>439</v>
+      </c>
+      <c r="B14" t="s">
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -2105,34 +2774,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" t="s">
         <v>138</v>
-      </c>
-      <c r="B2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" t="s">
         <v>212</v>
-      </c>
-      <c r="B3" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>276</v>
+      </c>
+      <c r="B4" t="s">
         <v>277</v>
-      </c>
-      <c r="B4" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B5" t="s">
         <v>283</v>
-      </c>
-      <c r="B5" t="s">
-        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -2142,15 +2811,15 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A034C685-69FA-4487-B3BF-C7BF8E932720}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.08984375" customWidth="1"/>
+    <col min="1" max="1" width="28.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -2203,98 +2872,154 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" t="s">
         <v>124</v>
-      </c>
-      <c r="B7" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B10" t="s">
         <v>175</v>
-      </c>
-      <c r="B10" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" t="s">
         <v>182</v>
-      </c>
-      <c r="B11" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B12" t="s">
         <v>186</v>
-      </c>
-      <c r="B12" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B13" t="s">
         <v>188</v>
-      </c>
-      <c r="B13" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>241</v>
+      </c>
+      <c r="B14" t="s">
         <v>242</v>
-      </c>
-      <c r="B14" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>280</v>
+      </c>
+      <c r="B15" t="s">
         <v>281</v>
-      </c>
-      <c r="B15" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B17" t="s">
-        <v>321</v>
+        <v>446</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B18" t="s">
-        <v>330</v>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>338</v>
+      </c>
+      <c r="B19" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>348</v>
+      </c>
+      <c r="B20" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>419</v>
+      </c>
+      <c r="B21" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>421</v>
+      </c>
+      <c r="B22" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>422</v>
+      </c>
+      <c r="B23" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>435</v>
+      </c>
+      <c r="B24" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>474</v>
+      </c>
+      <c r="B25" t="s">
+        <v>475</v>
       </c>
     </row>
   </sheetData>
@@ -2304,10 +3029,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46AD149B-B65F-49C4-AF01-021394194CC2}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2413,34 +3138,98 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B13" t="s">
         <v>196</v>
-      </c>
-      <c r="B13" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>225</v>
+      </c>
+      <c r="B14" t="s">
         <v>226</v>
-      </c>
-      <c r="B14" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>290</v>
+      </c>
+      <c r="B15" t="s">
         <v>291</v>
-      </c>
-      <c r="B15" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B16" t="s">
-        <v>328</v>
+        <v>325</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>351</v>
+      </c>
+      <c r="B17" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>355</v>
+      </c>
+      <c r="B18" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>387</v>
+      </c>
+      <c r="B19" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>388</v>
+      </c>
+      <c r="B20" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>390</v>
+      </c>
+      <c r="B21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>394</v>
+      </c>
+      <c r="B22" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>443</v>
+      </c>
+      <c r="B23" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>454</v>
+      </c>
+      <c r="B24" t="s">
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -2450,10 +3239,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{089252DC-DCE6-4CB7-BBC3-520320D586D5}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2503,7 +3292,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B6" t="s">
         <v>112</v>
@@ -2511,26 +3300,50 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>278</v>
+      </c>
+      <c r="B7" t="s">
         <v>279</v>
-      </c>
-      <c r="B7" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>293</v>
+      </c>
+      <c r="B8" t="s">
         <v>294</v>
-      </c>
-      <c r="B8" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B9" t="s">
-        <v>309</v>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>363</v>
+      </c>
+      <c r="B10" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>383</v>
+      </c>
+      <c r="B11" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>468</v>
+      </c>
+      <c r="B12" t="s">
+        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -2563,15 +3376,15 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE7B48C-6A57-4A65-BCF2-21AE9AC194C5}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -2584,10 +3397,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" t="s">
         <v>128</v>
       </c>
-      <c r="B2" t="s">
-        <v>129</v>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>424</v>
+      </c>
+      <c r="B4" t="s">
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -2597,10 +3426,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B164AC79-ACD3-4710-934B-FB8241A3324F}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2642,7 +3471,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
@@ -2650,42 +3479,66 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" t="s">
         <v>136</v>
-      </c>
-      <c r="B6" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B7" t="s">
         <v>214</v>
-      </c>
-      <c r="B7" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" t="s">
         <v>216</v>
-      </c>
-      <c r="B8" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>217</v>
+      </c>
+      <c r="B9" t="s">
         <v>218</v>
-      </c>
-      <c r="B9" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>227</v>
+      </c>
+      <c r="B10" t="s">
         <v>228</v>
       </c>
-      <c r="B10" t="s">
-        <v>229</v>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>430</v>
+      </c>
+      <c r="B11" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>453</v>
+      </c>
+      <c r="B12" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>470</v>
+      </c>
+      <c r="B13" t="s">
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -2739,10 +3592,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" t="s">
         <v>220</v>
-      </c>
-      <c r="B2" t="s">
-        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2775,15 +3628,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B5D6BBD-6DA2-42DF-A06F-6A55D030943B}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.08984375" customWidth="1"/>
+    <col min="1" max="1" width="23.6328125" customWidth="1"/>
     <col min="2" max="2" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2816,7 +3669,7 @@
         <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2845,34 +3698,98 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" t="s">
         <v>179</v>
-      </c>
-      <c r="B9" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B10" t="s">
         <v>253</v>
-      </c>
-      <c r="B10" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B11" t="s">
-        <v>315</v>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>336</v>
+      </c>
+      <c r="B12" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>369</v>
+      </c>
+      <c r="B13" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>371</v>
+      </c>
+      <c r="B14" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>373</v>
+      </c>
+      <c r="B15" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>378</v>
+      </c>
+      <c r="B16" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>392</v>
+      </c>
+      <c r="B17" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>395</v>
+      </c>
+      <c r="B18" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>456</v>
+      </c>
+      <c r="B19" t="s">
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -2883,10 +3800,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE90B0CB-4A82-4A75-95AE-F3C98AA6F040}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2945,106 +3862,130 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" t="s">
         <v>131</v>
-      </c>
-      <c r="B7" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" t="s">
         <v>158</v>
-      </c>
-      <c r="B8" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B10" t="s">
         <v>190</v>
-      </c>
-      <c r="B10" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" t="s">
         <v>194</v>
-      </c>
-      <c r="B11" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>199</v>
+      </c>
+      <c r="B12" t="s">
         <v>200</v>
-      </c>
-      <c r="B12" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>203</v>
+      </c>
+      <c r="B13" t="s">
         <v>204</v>
-      </c>
-      <c r="B13" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>245</v>
+      </c>
+      <c r="B14" t="s">
         <v>246</v>
-      </c>
-      <c r="B14" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>247</v>
+      </c>
+      <c r="B15" t="s">
         <v>248</v>
-      </c>
-      <c r="B15" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>254</v>
+      </c>
+      <c r="B16" t="s">
         <v>255</v>
-      </c>
-      <c r="B16" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>299</v>
+      </c>
+      <c r="B18" t="s">
         <v>300</v>
-      </c>
-      <c r="B18" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B19" t="s">
-        <v>309</v>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>400</v>
+      </c>
+      <c r="B20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>415</v>
+      </c>
+      <c r="B22" t="s">
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -3054,10 +3995,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA704C1C-49E1-499F-BBE3-96E07D259E79}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3072,18 +4013,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" t="s">
         <v>160</v>
-      </c>
-      <c r="B2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B3" t="s">
-        <v>312</v>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>381</v>
+      </c>
+      <c r="B4" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>401</v>
+      </c>
+      <c r="B5" t="s">
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -3094,10 +4051,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C20B180-3B4C-4969-A7B5-2323B0CBFDFD}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3139,26 +4096,58 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" t="s">
         <v>162</v>
-      </c>
-      <c r="B5" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>256</v>
+      </c>
+      <c r="B6" t="s">
         <v>257</v>
-      </c>
-      <c r="B6" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>284</v>
+      </c>
+      <c r="B7" t="s">
         <v>285</v>
       </c>
-      <c r="B7" t="s">
-        <v>286</v>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>328</v>
+      </c>
+      <c r="B8" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B9" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>428</v>
+      </c>
+      <c r="B10" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>449</v>
+      </c>
+      <c r="B11" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -3168,10 +4157,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2B4D34-5DD5-462B-BE1D-EDB156A99AAB}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3221,50 +4210,82 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" t="s">
         <v>152</v>
-      </c>
-      <c r="B6" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>205</v>
+      </c>
+      <c r="B7" t="s">
         <v>206</v>
-      </c>
-      <c r="B7" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B8" t="s">
         <v>232</v>
-      </c>
-      <c r="B8" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>250</v>
+      </c>
+      <c r="B10" t="s">
         <v>251</v>
-      </c>
-      <c r="B10" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>288</v>
+      </c>
+      <c r="B11" t="s">
         <v>289</v>
       </c>
-      <c r="B11" t="s">
-        <v>290</v>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>367</v>
+      </c>
+      <c r="B12" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>445</v>
+      </c>
+      <c r="B13" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>458</v>
+      </c>
+      <c r="B14" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>472</v>
+      </c>
+      <c r="B15" t="s">
+        <v>473</v>
       </c>
     </row>
   </sheetData>
@@ -3274,15 +4295,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1954444E-13D8-4952-9766-0067571A9DEC}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.90625" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -3359,90 +4380,130 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" t="s">
         <v>133</v>
-      </c>
-      <c r="B10" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" t="s">
         <v>146</v>
-      </c>
-      <c r="B11" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B12" t="s">
         <v>148</v>
-      </c>
-      <c r="B12" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" t="s">
         <v>164</v>
-      </c>
-      <c r="B13" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" t="s">
         <v>171</v>
-      </c>
-      <c r="B16" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B18" t="s">
         <v>202</v>
-      </c>
-      <c r="B18" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B19" t="s">
         <v>259</v>
-      </c>
-      <c r="B19" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>295</v>
+      </c>
+      <c r="B20" t="s">
         <v>296</v>
       </c>
-      <c r="B20" t="s">
-        <v>297</v>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>397</v>
+      </c>
+      <c r="B21" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>399</v>
+      </c>
+      <c r="B22" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>403</v>
+      </c>
+      <c r="B23" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>405</v>
+      </c>
+      <c r="B24" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>451</v>
+      </c>
+      <c r="B25" t="s">
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -3452,15 +4513,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF830CD-7188-43CF-8442-1E032F6FA383}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="1" max="1" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -3476,47 +4537,63 @@
         <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" t="s">
         <v>198</v>
-      </c>
-      <c r="B4" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B5" t="s">
         <v>236</v>
-      </c>
-      <c r="B5" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B7" t="s">
-        <v>223</v>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>409</v>
+      </c>
+      <c r="B8" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B9" t="s">
+        <v>412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>